<commit_message>
Add my Python Pandas out of my Jupyter notebook.
</commit_message>
<xml_diff>
--- a/Project_LibraryAnalysis_TaskManager.xlsx
+++ b/Project_LibraryAnalysis_TaskManager.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwmcgee\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwmcgee\Documents\Bootcamp\Projects\Rutgers-Data-Science-Bootcamp-Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40AA4E8-7830-4193-BFAA-C7971215C013}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5F52B4-C467-488D-B015-032CF3606434}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F151FD91-370E-49B8-9F8E-6368E44A0B3D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>TASK</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Create Field; Concatenate checkout month and year.</t>
   </si>
   <si>
-    <t>Limit data set to 10 years.</t>
-  </si>
-  <si>
     <t>Exclude unneccesary columns.</t>
   </si>
   <si>
@@ -109,6 +106,12 @@
   </si>
   <si>
     <t>Data Analysis</t>
+  </si>
+  <si>
+    <t>Limit data set to 5 years.</t>
+  </si>
+  <si>
+    <t>Remove duplicates.</t>
   </si>
 </sst>
 </file>
@@ -494,11 +497,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E5B195-44F8-4F76-A051-29566878D566}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +534,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -541,7 +544,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -551,7 +554,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -561,7 +564,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -571,7 +574,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -581,7 +584,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -591,7 +594,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -601,124 +604,124 @@
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>20</v>
@@ -727,8 +730,12 @@
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="4"/>
+      <c r="A22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
@@ -805,7 +812,10 @@
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="4"/>
       <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="C36" s="2"/>
@@ -819,9 +829,12 @@
     <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="C39" s="2"/>
     </row>
+    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="C40" s="2"/>
+    </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C39" xr:uid="{9A2A0BAC-6A0A-4408-B33B-9E58304687B4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C40" xr:uid="{9A2A0BAC-6A0A-4408-B33B-9E58304687B4}">
       <formula1>"KB,VJ,HP,JM"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>